<commit_message>
DatabaseExcel v1.1 PromotionTable & FAQTable added
</commit_message>
<xml_diff>
--- a/TravelDatabase.xlsx
+++ b/TravelDatabase.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\comp3111travelAgent\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10605" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10605" windowHeight="7635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tour List" sheetId="1" r:id="rId1"/>
-    <sheet name="Booking Table" sheetId="2" r:id="rId2"/>
-    <sheet name="Customer Table" sheetId="3" r:id="rId3"/>
+    <sheet name="FAQ" sheetId="4" r:id="rId2"/>
+    <sheet name="Promotion Table" sheetId="5" r:id="rId3"/>
+    <sheet name="Booking Table" sheetId="2" r:id="rId4"/>
+    <sheet name="Customer Table" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="289">
   <si>
     <t>China Guangdong Tour</t>
   </si>
@@ -791,6 +793,109 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to apply? </t>
+  </si>
+  <si>
+    <t>Question_no</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Customers shall approach the company by phone or visit our store (in Clearwater bay) with the choosen tour code and departure date. If it is not full, customers will be advised by the staff to pay the tour fee. Tour fee is non refundable. Customer can pay their fee by ATM to 123-345-432-211 of ABC Bank or by cash in our store. Customer shall send their pay-in slip to us by email or LINE.</t>
+  </si>
+  <si>
+    <t>Where is the gathering/assemble and dismiss spot?</t>
+  </si>
+  <si>
+    <t>What if the tour is cancelled?</t>
+  </si>
+  <si>
+    <t>In case a tour has not enough people or bad weather condition and the tour is forced to cancel, customers will be informed 3 days in advanced. Either change to another tour or refund is avaliable for customers to select. However, due to other reasons such as customers' personal problem no refund can be made.
+Are there any additional charge?</t>
+  </si>
+  <si>
+    <t>We gather at the gathering spot "Exit A, Futian port, Shenzhen" at 8:00AM on the departure date. We dismiss at the same spot after the tour. (see the picture gather.jpg)</t>
+  </si>
+  <si>
+    <t>Each customer need to pay an additional service charge at the rate $60/day/person, on top of the tour fee. It is collected by the tour guide at the end of the tour.</t>
+  </si>
+  <si>
+    <t>A tour bus</t>
+  </si>
+  <si>
+    <t>Each tour guide has a LINE account and he will add the customers as his friends before the departure date. You can contact him/her accordingly.</t>
+  </si>
+  <si>
+    <t>Yes, each customers are protected by the Excellent Blue-Diamond Scheme by AAA insurance company.</t>
+  </si>
+  <si>
+    <t>All rooms are twin beds. Every customer needs to share a room with another customer. If a customer prefer to own a room by himself/herself, additional charge of 30% will be applied.</t>
+  </si>
+  <si>
+    <t>Please refer the Visa issue to the immigration department of China. The tour are assembled and dismissed in mainland and no cross-border is needed. However, you will need a travelling document when you check in the hotel.</t>
+  </si>
+  <si>
+    <t>Yes you do need it. Otherwise you may not use the facility.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Age below 3 (including 3) is free. Age between 4 to 11 (including 4 and 11) has a discount of 20% off. Otherwise full fee applies. The same service charge is applied to all age customers</t>
+  </si>
+  <si>
+    <t>You shall contact the tour guide if you know you will be late and see if the tour guide can wait a little bit longer. No refund or make up shall be made if a customer is late for the tour.</t>
+  </si>
+  <si>
+    <t>Are there any additional charge?</t>
+  </si>
+  <si>
+    <t>What is the transportation in Guangdong?</t>
+  </si>
+  <si>
+    <t>How can I contact the tour guide?</t>
+  </si>
+  <si>
+    <t>Is insurance covered?</t>
+  </si>
+  <si>
+    <t>Is the hotel single bed or twin bed or double bed?</t>
+  </si>
+  <si>
+    <t>Visa problem</t>
+  </si>
+  <si>
+    <t>Do I need swimming suit in a water them park or a hot spring resort?</t>
+  </si>
+  <si>
+    <t>Do you serve vegeterian?</t>
+  </si>
+  <si>
+    <t>What is the tour fee for children?</t>
+  </si>
+  <si>
+    <t>What if I am late in the departure date?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tour ID </t>
+  </si>
+  <si>
+    <t>promotion_start</t>
+  </si>
+  <si>
+    <t>promotion_end</t>
+  </si>
+  <si>
+    <t>promotion_dec</t>
+  </si>
+  <si>
+    <t>discount</t>
   </si>
 </sst>
 </file>
@@ -800,7 +905,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;HK$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -864,6 +969,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -981,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1059,16 +1170,32 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1362,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C59" activeCellId="17" sqref="C7 C9 C13 C18 C22 C27 C30 C4 C36 C38 C41 C42 C45 C50 C53 C56 C57 C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1385,10 +1512,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="25.5" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1">
@@ -2625,10 +2752,10 @@
       <c r="P31" s="13"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="44"/>
+      <c r="B32" s="46"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
@@ -3165,10 +3292,10 @@
       <c r="P46" s="13"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="44"/>
+      <c r="B47" s="46"/>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
@@ -3730,9 +3857,644 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="32.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+    </row>
+    <row r="2" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="47">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+    </row>
+    <row r="3" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="47">
+        <v>2</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+    </row>
+    <row r="4" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="47">
+        <v>3</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+    </row>
+    <row r="5" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="47">
+        <v>4</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+    </row>
+    <row r="6" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="47">
+        <v>5</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+    </row>
+    <row r="7" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="47">
+        <v>6</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+    </row>
+    <row r="8" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="47">
+        <v>7</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+    </row>
+    <row r="9" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="47">
+        <v>8</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+    </row>
+    <row r="10" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="47">
+        <v>9</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+    </row>
+    <row r="11" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="47">
+        <v>10</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+    </row>
+    <row r="12" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="47">
+        <v>11</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+    </row>
+    <row r="13" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="47">
+        <v>12</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+    </row>
+    <row r="14" spans="1:14" s="38" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="47">
+        <v>13</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="52">
+        <v>43030</v>
+      </c>
+      <c r="C2" s="52">
+        <v>43050</v>
+      </c>
+      <c r="D2" s="42">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="52">
+        <v>43030</v>
+      </c>
+      <c r="C3" s="52">
+        <v>43050</v>
+      </c>
+      <c r="D3" s="42">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="52">
+        <v>43030</v>
+      </c>
+      <c r="C4" s="52">
+        <v>43050</v>
+      </c>
+      <c r="D4" s="42">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="52">
+        <v>43030</v>
+      </c>
+      <c r="C5" s="52">
+        <v>43050</v>
+      </c>
+      <c r="D5" s="42">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="52">
+        <v>43032</v>
+      </c>
+      <c r="C6" s="52">
+        <v>43052</v>
+      </c>
+      <c r="D6" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="52">
+        <v>43032</v>
+      </c>
+      <c r="C7" s="52">
+        <v>43052</v>
+      </c>
+      <c r="D7" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="52">
+        <v>43032</v>
+      </c>
+      <c r="C8" s="52">
+        <v>43052</v>
+      </c>
+      <c r="D8" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="52">
+        <v>43036</v>
+      </c>
+      <c r="C9" s="52">
+        <v>43056</v>
+      </c>
+      <c r="D9" s="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="52">
+        <v>43036</v>
+      </c>
+      <c r="C10" s="52">
+        <v>43056</v>
+      </c>
+      <c r="D10" s="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="52">
+        <v>43036</v>
+      </c>
+      <c r="C11" s="52">
+        <v>43056</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="52">
+        <v>43038</v>
+      </c>
+      <c r="C12" s="52">
+        <v>43058</v>
+      </c>
+      <c r="D12" s="42">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="52">
+        <v>43040</v>
+      </c>
+      <c r="C13" s="52">
+        <v>43060</v>
+      </c>
+      <c r="D13" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="52">
+        <v>43040</v>
+      </c>
+      <c r="C14" s="52">
+        <v>43060</v>
+      </c>
+      <c r="D14" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="52">
+        <v>43040</v>
+      </c>
+      <c r="C15" s="52">
+        <v>43060</v>
+      </c>
+      <c r="D15" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="52">
+        <v>43040</v>
+      </c>
+      <c r="C16" s="52">
+        <v>43060</v>
+      </c>
+      <c r="D16" s="42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="52">
+        <v>43041</v>
+      </c>
+      <c r="C17" s="52">
+        <v>43063</v>
+      </c>
+      <c r="D17" s="42">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" s="52">
+        <v>43041</v>
+      </c>
+      <c r="C18" s="52">
+        <v>43061</v>
+      </c>
+      <c r="D18" s="42">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="52">
+        <v>43041</v>
+      </c>
+      <c r="C19" s="52">
+        <v>43061</v>
+      </c>
+      <c r="D19" s="42">
+        <v>0.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -3745,7 +4507,7 @@
     <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.25" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.25" style="44" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.875" bestFit="1" customWidth="1"/>
@@ -3780,7 +4542,7 @@
       <c r="G2" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="43" t="s">
         <v>193</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -3817,7 +4579,7 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="44">
         <f>VLOOKUP($D3,'Tour List'!$C$2:$K$60,9,0)*$E3+VLOOKUP($D3,'Tour List'!$C$2:$K$60,9,0)*$F3*0.8</f>
         <v>798</v>
       </c>
@@ -3845,7 +4607,7 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="44">
         <f>VLOOKUP($D4,'Tour List'!$C$2:$K$60,9,0)*$E4+VLOOKUP($D4,'Tour List'!$C$2:$K$60,9,0)*$F4*0.8</f>
         <v>14396.400000000001</v>
       </c>
@@ -3873,7 +4635,7 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="44">
         <f>VLOOKUP($D5,'Tour List'!$C$2:$K$60,9,0)*$E5+VLOOKUP($D5,'Tour List'!$C$2:$K$60,9,0)*$F5*0.8</f>
         <v>2097</v>
       </c>
@@ -3901,7 +4663,7 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="44">
         <f>VLOOKUP($D6,'Tour List'!$C$2:$K$60,9,0)*$E6+VLOOKUP($D6,'Tour List'!$C$2:$K$60,9,0)*$F6*0.8</f>
         <v>898.2</v>
       </c>
@@ -3929,7 +4691,7 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="44">
         <f>VLOOKUP($D7,'Tour List'!$C$2:$K$60,9,0)*$E7+VLOOKUP($D7,'Tour List'!$C$2:$K$60,9,0)*$F7*0.8</f>
         <v>799</v>
       </c>
@@ -3957,7 +4719,7 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="44">
         <f>VLOOKUP($D8,'Tour List'!$C$2:$K$60,9,0)*$E8+VLOOKUP($D8,'Tour List'!$C$2:$K$60,9,0)*$F8*0.8</f>
         <v>2097</v>
       </c>
@@ -3985,7 +4747,7 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="44">
         <f>VLOOKUP($D9,'Tour List'!$C$2:$K$60,9,0)*$E9+VLOOKUP($D9,'Tour List'!$C$2:$K$60,9,0)*$F9*0.8</f>
         <v>5597.2</v>
       </c>
@@ -4013,7 +4775,7 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="44">
         <f>VLOOKUP($D10,'Tour List'!$C$2:$K$60,9,0)*$E10+VLOOKUP($D10,'Tour List'!$C$2:$K$60,9,0)*$F10*0.8</f>
         <v>35996</v>
       </c>
@@ -4041,7 +4803,7 @@
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="44">
         <f>VLOOKUP($D11,'Tour List'!$C$2:$K$60,9,0)*$E11+VLOOKUP($D11,'Tour List'!$C$2:$K$60,9,0)*$F11*0.8</f>
         <v>3699</v>
       </c>
@@ -4069,7 +4831,7 @@
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="44">
         <f>VLOOKUP($D12,'Tour List'!$C$2:$K$60,9,0)*$E12+VLOOKUP($D12,'Tour List'!$C$2:$K$60,9,0)*$F12*0.8</f>
         <v>8636.4</v>
       </c>
@@ -4097,7 +4859,7 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="44">
         <f>VLOOKUP($D13,'Tour List'!$C$2:$K$60,9,0)*$E13+VLOOKUP($D13,'Tour List'!$C$2:$K$60,9,0)*$F13*0.8</f>
         <v>499</v>
       </c>
@@ -4125,7 +4887,7 @@
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="44">
         <f>VLOOKUP($D14,'Tour List'!$C$2:$K$60,9,0)*$E14+VLOOKUP($D14,'Tour List'!$C$2:$K$60,9,0)*$F14*0.8</f>
         <v>1996</v>
       </c>
@@ -4153,7 +4915,7 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="H15" s="46">
+      <c r="H15" s="44">
         <f>VLOOKUP($D15,'Tour List'!$C$2:$K$60,9,0)*$E15+VLOOKUP($D15,'Tour List'!$C$2:$K$60,9,0)*$F15*0.8</f>
         <v>1397.2</v>
       </c>
@@ -4181,7 +4943,7 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="H16" s="46">
+      <c r="H16" s="44">
         <f>VLOOKUP($D16,'Tour List'!$C$2:$K$60,9,0)*$E16+VLOOKUP($D16,'Tour List'!$C$2:$K$60,9,0)*$F16*0.8</f>
         <v>299</v>
       </c>
@@ -4209,7 +4971,7 @@
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="H17" s="46">
+      <c r="H17" s="44">
         <f>VLOOKUP($D17,'Tour List'!$C$2:$K$60,9,0)*$E17+VLOOKUP($D17,'Tour List'!$C$2:$K$60,9,0)*$F17*0.8</f>
         <v>2999</v>
       </c>
@@ -4237,7 +4999,7 @@
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="H18" s="46">
+      <c r="H18" s="44">
         <f>VLOOKUP($D18,'Tour List'!$C$2:$K$60,9,0)*$E18+VLOOKUP($D18,'Tour List'!$C$2:$K$60,9,0)*$F18*0.8</f>
         <v>7197</v>
       </c>
@@ -4265,7 +5027,7 @@
       <c r="F19">
         <v>1</v>
       </c>
-      <c r="H19" s="46">
+      <c r="H19" s="44">
         <f>VLOOKUP($D19,'Tour List'!$C$2:$K$60,9,0)*$E19+VLOOKUP($D19,'Tour List'!$C$2:$K$60,9,0)*$F19*0.8</f>
         <v>898.2</v>
       </c>
@@ -4293,7 +5055,7 @@
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="H20" s="46">
+      <c r="H20" s="44">
         <f>VLOOKUP($D20,'Tour List'!$C$2:$K$60,9,0)*$E20+VLOOKUP($D20,'Tour List'!$C$2:$K$60,9,0)*$F20*0.8</f>
         <v>17998</v>
       </c>
@@ -4321,7 +5083,7 @@
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="H21" s="46">
+      <c r="H21" s="44">
         <f>VLOOKUP($D21,'Tour List'!$C$2:$K$60,9,0)*$E21+VLOOKUP($D21,'Tour List'!$C$2:$K$60,9,0)*$F21*0.8</f>
         <v>15998</v>
       </c>
@@ -4349,7 +5111,7 @@
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="H22" s="46">
+      <c r="H22" s="44">
         <f>VLOOKUP($D22,'Tour List'!$C$2:$K$60,9,0)*$E22+VLOOKUP($D22,'Tour List'!$C$2:$K$60,9,0)*$F22*0.8</f>
         <v>897</v>
       </c>
@@ -4377,7 +5139,7 @@
       <c r="F23">
         <v>2</v>
       </c>
-      <c r="H23" s="46">
+      <c r="H23" s="44">
         <f>VLOOKUP($D23,'Tour List'!$C$2:$K$60,9,0)*$E23+VLOOKUP($D23,'Tour List'!$C$2:$K$60,9,0)*$F23*0.8</f>
         <v>2516.4</v>
       </c>
@@ -4405,7 +5167,7 @@
       <c r="F24">
         <v>0</v>
       </c>
-      <c r="H24" s="46">
+      <c r="H24" s="44">
         <f>VLOOKUP($D24,'Tour List'!$C$2:$K$60,9,0)*$E24+VLOOKUP($D24,'Tour List'!$C$2:$K$60,9,0)*$F24*0.8</f>
         <v>499</v>
       </c>
@@ -4433,7 +5195,7 @@
       <c r="F25">
         <v>0</v>
       </c>
-      <c r="H25" s="46">
+      <c r="H25" s="44">
         <f>VLOOKUP($D25,'Tour List'!$C$2:$K$60,9,0)*$E25+VLOOKUP($D25,'Tour List'!$C$2:$K$60,9,0)*$F25*0.8</f>
         <v>7999</v>
       </c>
@@ -4461,7 +5223,7 @@
       <c r="F26">
         <v>0</v>
       </c>
-      <c r="H26" s="46">
+      <c r="H26" s="44">
         <f>VLOOKUP($D26,'Tour List'!$C$2:$K$60,9,0)*$E26+VLOOKUP($D26,'Tour List'!$C$2:$K$60,9,0)*$F26*0.8</f>
         <v>5998</v>
       </c>
@@ -4489,7 +5251,7 @@
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="H27" s="46">
+      <c r="H27" s="44">
         <f>VLOOKUP($D27,'Tour List'!$C$2:$K$60,9,0)*$E27+VLOOKUP($D27,'Tour List'!$C$2:$K$60,9,0)*$F27*0.8</f>
         <v>13157.2</v>
       </c>
@@ -4517,7 +5279,7 @@
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="H28" s="46">
+      <c r="H28" s="44">
         <f>VLOOKUP($D28,'Tour List'!$C$2:$K$60,9,0)*$E28+VLOOKUP($D28,'Tour List'!$C$2:$K$60,9,0)*$F28*0.8</f>
         <v>25197</v>
       </c>
@@ -4545,7 +5307,7 @@
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="H29" s="46">
+      <c r="H29" s="44">
         <f>VLOOKUP($D29,'Tour List'!$C$2:$K$60,9,0)*$E29+VLOOKUP($D29,'Tour List'!$C$2:$K$60,9,0)*$F29*0.8</f>
         <v>1798</v>
       </c>
@@ -4573,7 +5335,7 @@
       <c r="F30">
         <v>2</v>
       </c>
-      <c r="H30" s="46">
+      <c r="H30" s="44">
         <f>VLOOKUP($D30,'Tour List'!$C$2:$K$60,9,0)*$E30+VLOOKUP($D30,'Tour List'!$C$2:$K$60,9,0)*$F30*0.8</f>
         <v>777.40000000000009</v>
       </c>
@@ -4601,7 +5363,7 @@
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="H31" s="46">
+      <c r="H31" s="44">
         <f>VLOOKUP($D31,'Tour List'!$C$2:$K$60,9,0)*$E31+VLOOKUP($D31,'Tour List'!$C$2:$K$60,9,0)*$F31*0.8</f>
         <v>598</v>
       </c>
@@ -4629,7 +5391,7 @@
       <c r="F32">
         <v>0</v>
       </c>
-      <c r="H32" s="46">
+      <c r="H32" s="44">
         <f>VLOOKUP($D32,'Tour List'!$C$2:$K$60,9,0)*$E32+VLOOKUP($D32,'Tour List'!$C$2:$K$60,9,0)*$F32*0.8</f>
         <v>14997</v>
       </c>
@@ -4657,7 +5419,7 @@
       <c r="F33">
         <v>0</v>
       </c>
-      <c r="H33" s="46">
+      <c r="H33" s="44">
         <f>VLOOKUP($D33,'Tour List'!$C$2:$K$60,9,0)*$E33+VLOOKUP($D33,'Tour List'!$C$2:$K$60,9,0)*$F33*0.8</f>
         <v>1196</v>
       </c>
@@ -4685,7 +5447,7 @@
       <c r="F34">
         <v>0</v>
       </c>
-      <c r="H34" s="46">
+      <c r="H34" s="44">
         <f>VLOOKUP($D34,'Tour List'!$C$2:$K$60,9,0)*$E34+VLOOKUP($D34,'Tour List'!$C$2:$K$60,9,0)*$F34*0.8</f>
         <v>998</v>
       </c>
@@ -4713,7 +5475,7 @@
       <c r="F35">
         <v>1</v>
       </c>
-      <c r="H35" s="46">
+      <c r="H35" s="44">
         <f>VLOOKUP($D35,'Tour List'!$C$2:$K$60,9,0)*$E35+VLOOKUP($D35,'Tour List'!$C$2:$K$60,9,0)*$F35*0.8</f>
         <v>898.2</v>
       </c>
@@ -4741,7 +5503,7 @@
       <c r="F36">
         <v>0</v>
       </c>
-      <c r="H36" s="46">
+      <c r="H36" s="44">
         <f>VLOOKUP($D36,'Tour List'!$C$2:$K$60,9,0)*$E36+VLOOKUP($D36,'Tour List'!$C$2:$K$60,9,0)*$F36*0.8</f>
         <v>1398</v>
       </c>
@@ -4769,7 +5531,7 @@
       <c r="F37">
         <v>0</v>
       </c>
-      <c r="H37" s="46">
+      <c r="H37" s="44">
         <f>VLOOKUP($D37,'Tour List'!$C$2:$K$60,9,0)*$E37+VLOOKUP($D37,'Tour List'!$C$2:$K$60,9,0)*$F37*0.8</f>
         <v>19197</v>
       </c>
@@ -4797,7 +5559,7 @@
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="H38" s="46">
+      <c r="H38" s="44">
         <f>VLOOKUP($D38,'Tour List'!$C$2:$K$60,9,0)*$E38+VLOOKUP($D38,'Tour List'!$C$2:$K$60,9,0)*$F38*0.8</f>
         <v>6699</v>
       </c>
@@ -4825,7 +5587,7 @@
       <c r="F39">
         <v>0</v>
       </c>
-      <c r="H39" s="46">
+      <c r="H39" s="44">
         <f>VLOOKUP($D39,'Tour List'!$C$2:$K$60,9,0)*$E39+VLOOKUP($D39,'Tour List'!$C$2:$K$60,9,0)*$F39*0.8</f>
         <v>1198</v>
       </c>
@@ -4853,7 +5615,7 @@
       <c r="F40">
         <v>0</v>
       </c>
-      <c r="H40" s="46">
+      <c r="H40" s="44">
         <f>VLOOKUP($D40,'Tour List'!$C$2:$K$60,9,0)*$E40+VLOOKUP($D40,'Tour List'!$C$2:$K$60,9,0)*$F40*0.8</f>
         <v>19197</v>
       </c>
@@ -4881,7 +5643,7 @@
       <c r="F41">
         <v>0</v>
       </c>
-      <c r="H41" s="46">
+      <c r="H41" s="44">
         <f>VLOOKUP($D41,'Tour List'!$C$2:$K$60,9,0)*$E41+VLOOKUP($D41,'Tour List'!$C$2:$K$60,9,0)*$F41*0.8</f>
         <v>1398</v>
       </c>
@@ -4909,7 +5671,7 @@
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="H42" s="46">
+      <c r="H42" s="44">
         <f>VLOOKUP($D42,'Tour List'!$C$2:$K$60,9,0)*$E42+VLOOKUP($D42,'Tour List'!$C$2:$K$60,9,0)*$F42*0.8</f>
         <v>1618.2</v>
       </c>
@@ -4937,7 +5699,7 @@
       <c r="F43">
         <v>0</v>
       </c>
-      <c r="H43" s="46">
+      <c r="H43" s="44">
         <f>VLOOKUP($D43,'Tour List'!$C$2:$K$60,9,0)*$E43+VLOOKUP($D43,'Tour List'!$C$2:$K$60,9,0)*$F43*0.8</f>
         <v>3999</v>
       </c>
@@ -4965,7 +5727,7 @@
       <c r="F44">
         <v>3</v>
       </c>
-      <c r="H44" s="46">
+      <c r="H44" s="44">
         <f>VLOOKUP($D44,'Tour List'!$C$2:$K$60,9,0)*$E44+VLOOKUP($D44,'Tour List'!$C$2:$K$60,9,0)*$F44*0.8</f>
         <v>22776.6</v>
       </c>
@@ -4993,7 +5755,7 @@
       <c r="F45">
         <v>0</v>
       </c>
-      <c r="H45" s="46">
+      <c r="H45" s="44">
         <f>VLOOKUP($D45,'Tour List'!$C$2:$K$60,9,0)*$E45+VLOOKUP($D45,'Tour List'!$C$2:$K$60,9,0)*$F45*0.8</f>
         <v>13398</v>
       </c>
@@ -5021,7 +5783,7 @@
       <c r="F46">
         <v>0</v>
       </c>
-      <c r="H46" s="46">
+      <c r="H46" s="44">
         <f>VLOOKUP($D46,'Tour List'!$C$2:$K$60,9,0)*$E46+VLOOKUP($D46,'Tour List'!$C$2:$K$60,9,0)*$F46*0.8</f>
         <v>11398</v>
       </c>
@@ -5049,7 +5811,7 @@
       <c r="F47">
         <v>0</v>
       </c>
-      <c r="H47" s="46">
+      <c r="H47" s="44">
         <f>VLOOKUP($D47,'Tour List'!$C$2:$K$60,9,0)*$E47+VLOOKUP($D47,'Tour List'!$C$2:$K$60,9,0)*$F47*0.8</f>
         <v>17097</v>
       </c>
@@ -5077,7 +5839,7 @@
       <c r="F48">
         <v>0</v>
       </c>
-      <c r="H48" s="46">
+      <c r="H48" s="44">
         <f>VLOOKUP($D48,'Tour List'!$C$2:$K$60,9,0)*$E48+VLOOKUP($D48,'Tour List'!$C$2:$K$60,9,0)*$F48*0.8</f>
         <v>11398</v>
       </c>
@@ -5105,7 +5867,7 @@
       <c r="F49">
         <v>1</v>
       </c>
-      <c r="H49" s="46">
+      <c r="H49" s="44">
         <f>VLOOKUP($D49,'Tour List'!$C$2:$K$60,9,0)*$E49+VLOOKUP($D49,'Tour List'!$C$2:$K$60,9,0)*$F49*0.8</f>
         <v>10258.200000000001</v>
       </c>
@@ -5122,7 +5884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
DatabaseExcel v1.2 CountryTable/RegionTable/CustomerTable/AdminTable added
</commit_message>
<xml_diff>
--- a/TravelDatabase.xlsx
+++ b/TravelDatabase.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="359">
   <si>
     <t>China Guangdong Tour</t>
   </si>
@@ -1104,6 +1104,12 @@
   </si>
   <si>
     <t>pay_confirmed</t>
+  </si>
+  <si>
+    <t>７</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shikoku </t>
   </si>
 </sst>
 </file>
@@ -1181,21 +1187,24 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF212121"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1381,15 +1390,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1461,6 +1461,21 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1755,49 +1770,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.75" style="31" customWidth="1"/>
-    <col min="2" max="2" width="9" style="31" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.875" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" style="31" customWidth="1"/>
-    <col min="9" max="9" width="14.375" style="31" customWidth="1"/>
-    <col min="10" max="10" width="24" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.125" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" style="31"/>
-    <col min="13" max="13" width="20" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.375" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="31"/>
+    <col min="1" max="1" width="11.75" style="26" customWidth="1"/>
+    <col min="2" max="2" width="9" style="26" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.875" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="26" customWidth="1"/>
+    <col min="9" max="9" width="14.375" style="26" customWidth="1"/>
+    <col min="10" max="10" width="24" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.125" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="26"/>
+    <col min="13" max="13" width="20" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.375" style="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="25.5" customHeight="1">
-      <c r="A1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="51"/>
+      <c r="A1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46"/>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="28" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -1824,1232 +1839,1232 @@
       <c r="M2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="45" t="s">
         <v>355</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="31">
-        <v>1</v>
-      </c>
-      <c r="B3" s="31">
-        <v>1</v>
-      </c>
-      <c r="C3" s="31" t="s">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="27">
         <v>2</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="29">
         <v>43056</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="27">
         <v>20</v>
       </c>
-      <c r="J3" s="32">
+      <c r="J3" s="27">
         <v>4</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="30">
         <v>499</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="31">
-        <v>1</v>
-      </c>
-      <c r="B4" s="31">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31" t="s">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="26">
+        <v>1</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="27">
         <v>2</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="29">
         <v>43062</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="27">
         <v>20</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="27">
         <v>4</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K4" s="30">
         <v>499</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="31">
-        <v>1</v>
-      </c>
-      <c r="B5" s="31">
-        <v>1</v>
-      </c>
-      <c r="C5" s="31" t="s">
+      <c r="A5" s="26">
+        <v>1</v>
+      </c>
+      <c r="B5" s="26">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="27">
         <v>2</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="29">
         <v>43071</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="27">
         <v>20</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="27">
         <v>4</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="30">
         <v>599</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="31">
-        <v>1</v>
-      </c>
-      <c r="B6" s="31">
-        <v>1</v>
-      </c>
-      <c r="C6" s="36" t="s">
+      <c r="A6" s="26">
+        <v>1</v>
+      </c>
+      <c r="B6" s="26">
+        <v>1</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="32">
         <v>2</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="29">
         <v>43056</v>
       </c>
-      <c r="I6" s="37">
+      <c r="I6" s="32">
         <v>20</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="27">
         <v>4</v>
       </c>
-      <c r="K6" s="38">
+      <c r="K6" s="33">
         <v>299</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="31">
-        <v>1</v>
-      </c>
-      <c r="B7" s="31">
-        <v>1</v>
-      </c>
-      <c r="C7" s="36" t="s">
+      <c r="A7" s="26">
+        <v>1</v>
+      </c>
+      <c r="B7" s="26">
+        <v>1</v>
+      </c>
+      <c r="C7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="27">
         <v>2</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="29">
         <v>43062</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="32">
         <v>20</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="27">
         <v>4</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="34">
         <v>299</v>
       </c>
-      <c r="L7" s="40" t="s">
+      <c r="L7" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="M7" s="41"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="31">
-        <v>1</v>
-      </c>
-      <c r="B8" s="31">
-        <v>1</v>
-      </c>
-      <c r="C8" s="36" t="s">
+      <c r="A8" s="26">
+        <v>1</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1</v>
+      </c>
+      <c r="C8" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="27">
         <v>2</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="37">
         <v>43073</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="32">
         <v>20</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="27">
         <v>4</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="30">
         <v>299</v>
       </c>
-      <c r="L8" s="43" t="s">
+      <c r="L8" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="31">
-        <v>1</v>
-      </c>
-      <c r="B9" s="31">
-        <v>1</v>
-      </c>
-      <c r="C9" s="36" t="s">
+      <c r="A9" s="26">
+        <v>1</v>
+      </c>
+      <c r="B9" s="26">
+        <v>1</v>
+      </c>
+      <c r="C9" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="27">
         <v>2</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="29">
         <v>43056</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9" s="32">
         <v>20</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="27">
         <v>4</v>
       </c>
-      <c r="K9" s="38">
+      <c r="K9" s="33">
         <v>299</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="L9" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="31">
-        <v>1</v>
-      </c>
-      <c r="B10" s="31">
-        <v>1</v>
-      </c>
-      <c r="C10" s="36" t="s">
+      <c r="A10" s="26">
+        <v>1</v>
+      </c>
+      <c r="B10" s="26">
+        <v>1</v>
+      </c>
+      <c r="C10" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="27">
         <v>2</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="29">
         <v>43062</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="32">
         <v>20</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="27">
         <v>4</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="30">
         <v>299</v>
       </c>
-      <c r="L10" s="44" t="s">
+      <c r="L10" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="31">
-        <v>1</v>
-      </c>
-      <c r="B11" s="31">
-        <v>1</v>
-      </c>
-      <c r="C11" s="36" t="s">
+      <c r="A11" s="26">
+        <v>1</v>
+      </c>
+      <c r="B11" s="26">
+        <v>1</v>
+      </c>
+      <c r="C11" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="27">
         <v>2</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="29">
         <v>43071</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="32">
         <v>20</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="27">
         <v>4</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="30">
         <v>399</v>
       </c>
-      <c r="L11" s="45" t="s">
+      <c r="L11" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="31">
-        <v>1</v>
-      </c>
-      <c r="B12" s="31">
-        <v>1</v>
-      </c>
-      <c r="C12" s="31" t="s">
+      <c r="A12" s="26">
+        <v>1</v>
+      </c>
+      <c r="B12" s="26">
+        <v>1</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="27">
         <v>2</v>
       </c>
-      <c r="H12" s="34">
+      <c r="H12" s="29">
         <v>43060</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="32">
         <v>20</v>
       </c>
-      <c r="J12" s="32">
+      <c r="J12" s="27">
         <v>4</v>
       </c>
-      <c r="K12" s="38">
+      <c r="K12" s="33">
         <v>299</v>
       </c>
-      <c r="L12" s="46" t="s">
+      <c r="L12" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="31">
-        <v>1</v>
-      </c>
-      <c r="B13" s="31">
-        <v>1</v>
-      </c>
-      <c r="C13" s="31" t="s">
+      <c r="A13" s="26">
+        <v>1</v>
+      </c>
+      <c r="B13" s="26">
+        <v>1</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="27">
         <v>2</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="29">
         <v>43071</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="32">
         <v>20</v>
       </c>
-      <c r="J13" s="32">
+      <c r="J13" s="27">
         <v>4</v>
       </c>
-      <c r="K13" s="35">
+      <c r="K13" s="30">
         <v>399</v>
       </c>
-      <c r="L13" s="46" t="s">
+      <c r="L13" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="31">
-        <v>1</v>
-      </c>
-      <c r="B14" s="31">
-        <v>1</v>
-      </c>
-      <c r="C14" s="31" t="s">
+      <c r="A14" s="26">
+        <v>1</v>
+      </c>
+      <c r="B14" s="26">
+        <v>1</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="27">
         <v>2</v>
       </c>
-      <c r="H14" s="34">
+      <c r="H14" s="29">
         <v>43060</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="32">
         <v>20</v>
       </c>
-      <c r="J14" s="32">
+      <c r="J14" s="27">
         <v>4</v>
       </c>
-      <c r="K14" s="35">
+      <c r="K14" s="30">
         <v>399</v>
       </c>
-      <c r="L14" s="40" t="s">
+      <c r="L14" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="31">
-        <v>1</v>
-      </c>
-      <c r="B15" s="31">
-        <v>1</v>
-      </c>
-      <c r="C15" s="31" t="s">
+      <c r="A15" s="26">
+        <v>1</v>
+      </c>
+      <c r="B15" s="26">
+        <v>1</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="27">
         <v>2</v>
       </c>
-      <c r="H15" s="34">
+      <c r="H15" s="29">
         <v>43071</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15" s="32">
         <v>20</v>
       </c>
-      <c r="J15" s="32">
+      <c r="J15" s="27">
         <v>4</v>
       </c>
-      <c r="K15" s="35">
+      <c r="K15" s="30">
         <v>499</v>
       </c>
-      <c r="L15" s="40" t="s">
+      <c r="L15" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="M15" s="41"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="31">
-        <v>1</v>
-      </c>
-      <c r="B16" s="31">
-        <v>1</v>
-      </c>
-      <c r="C16" s="31" t="s">
+      <c r="A16" s="26">
+        <v>1</v>
+      </c>
+      <c r="B16" s="26">
+        <v>1</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="27">
         <v>3</v>
       </c>
-      <c r="H16" s="34">
+      <c r="H16" s="29">
         <v>43056</v>
       </c>
-      <c r="I16" s="47">
+      <c r="I16" s="42">
         <v>20</v>
       </c>
-      <c r="J16" s="32">
+      <c r="J16" s="27">
         <v>4</v>
       </c>
-      <c r="K16" s="35">
+      <c r="K16" s="30">
         <v>599</v>
       </c>
-      <c r="L16" s="44" t="s">
+      <c r="L16" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="M16" s="41"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="31">
-        <v>1</v>
-      </c>
-      <c r="B17" s="31">
-        <v>1</v>
-      </c>
-      <c r="C17" s="31" t="s">
+      <c r="A17" s="26">
+        <v>1</v>
+      </c>
+      <c r="B17" s="26">
+        <v>1</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="27">
         <v>3</v>
       </c>
-      <c r="H17" s="34">
+      <c r="H17" s="29">
         <v>43060</v>
       </c>
-      <c r="I17" s="37">
+      <c r="I17" s="32">
         <v>20</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="27">
         <v>4</v>
       </c>
-      <c r="K17" s="48">
+      <c r="K17" s="43">
         <v>599</v>
       </c>
-      <c r="L17" s="40" t="s">
+      <c r="L17" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="31">
-        <v>1</v>
-      </c>
-      <c r="B18" s="31">
-        <v>1</v>
-      </c>
-      <c r="C18" s="31" t="s">
+      <c r="A18" s="26">
+        <v>1</v>
+      </c>
+      <c r="B18" s="26">
+        <v>1</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="27">
         <v>3</v>
       </c>
-      <c r="H18" s="34">
+      <c r="H18" s="29">
         <v>43071</v>
       </c>
-      <c r="I18" s="37">
+      <c r="I18" s="32">
         <v>20</v>
       </c>
-      <c r="J18" s="32">
+      <c r="J18" s="27">
         <v>4</v>
       </c>
-      <c r="K18" s="48">
+      <c r="K18" s="43">
         <v>799</v>
       </c>
-      <c r="L18" s="46" t="s">
+      <c r="L18" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="31">
-        <v>1</v>
-      </c>
-      <c r="B19" s="31">
-        <v>1</v>
-      </c>
-      <c r="C19" s="31" t="s">
+      <c r="A19" s="26">
+        <v>1</v>
+      </c>
+      <c r="B19" s="26">
+        <v>1</v>
+      </c>
+      <c r="C19" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="27">
         <v>3</v>
       </c>
-      <c r="H19" s="34">
+      <c r="H19" s="29">
         <v>43056</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="42">
         <v>20</v>
       </c>
-      <c r="J19" s="32">
+      <c r="J19" s="27">
         <v>4</v>
       </c>
-      <c r="K19" s="48">
+      <c r="K19" s="43">
         <v>699</v>
       </c>
-      <c r="L19" s="40" t="s">
+      <c r="L19" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="31">
-        <v>1</v>
-      </c>
-      <c r="B20" s="31">
-        <v>1</v>
-      </c>
-      <c r="C20" s="31" t="s">
+      <c r="A20" s="26">
+        <v>1</v>
+      </c>
+      <c r="B20" s="26">
+        <v>1</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="27">
         <v>3</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="29">
         <v>43060</v>
       </c>
-      <c r="I20" s="47">
+      <c r="I20" s="42">
         <v>20</v>
       </c>
-      <c r="J20" s="32">
+      <c r="J20" s="27">
         <v>4</v>
       </c>
-      <c r="K20" s="48">
+      <c r="K20" s="43">
         <v>699</v>
       </c>
-      <c r="L20" s="40" t="s">
+      <c r="L20" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="31">
-        <v>1</v>
-      </c>
-      <c r="B21" s="31">
-        <v>1</v>
-      </c>
-      <c r="C21" s="31" t="s">
+      <c r="A21" s="26">
+        <v>1</v>
+      </c>
+      <c r="B21" s="26">
+        <v>1</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="27">
         <v>3</v>
       </c>
-      <c r="H21" s="34">
+      <c r="H21" s="29">
         <v>43071</v>
       </c>
-      <c r="I21" s="47">
+      <c r="I21" s="42">
         <v>20</v>
       </c>
-      <c r="J21" s="32">
+      <c r="J21" s="27">
         <v>4</v>
       </c>
-      <c r="K21" s="48">
+      <c r="K21" s="43">
         <v>899</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="31">
-        <v>1</v>
-      </c>
-      <c r="B22" s="31">
-        <v>1</v>
-      </c>
-      <c r="C22" s="31" t="s">
+      <c r="A22" s="26">
+        <v>1</v>
+      </c>
+      <c r="B22" s="26">
+        <v>1</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="37" t="s">
+      <c r="F22" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="27">
         <v>3</v>
       </c>
-      <c r="H22" s="34">
+      <c r="H22" s="29">
         <v>43056</v>
       </c>
-      <c r="I22" s="47">
+      <c r="I22" s="42">
         <v>20</v>
       </c>
-      <c r="J22" s="32">
+      <c r="J22" s="27">
         <v>4</v>
       </c>
-      <c r="K22" s="48">
+      <c r="K22" s="43">
         <v>499</v>
       </c>
-      <c r="L22" s="46" t="s">
+      <c r="L22" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="31">
-        <v>1</v>
-      </c>
-      <c r="B23" s="31">
-        <v>1</v>
-      </c>
-      <c r="C23" s="31" t="s">
+      <c r="A23" s="26">
+        <v>1</v>
+      </c>
+      <c r="B23" s="26">
+        <v>1</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="27">
         <v>3</v>
       </c>
-      <c r="H23" s="34">
+      <c r="H23" s="29">
         <v>43061</v>
       </c>
-      <c r="I23" s="47">
+      <c r="I23" s="42">
         <v>20</v>
       </c>
-      <c r="J23" s="32">
+      <c r="J23" s="27">
         <v>4</v>
       </c>
-      <c r="K23" s="48">
+      <c r="K23" s="43">
         <v>499</v>
       </c>
-      <c r="L23" s="46" t="s">
+      <c r="L23" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="31">
-        <v>1</v>
-      </c>
-      <c r="B24" s="31">
-        <v>1</v>
-      </c>
-      <c r="C24" s="31" t="s">
+      <c r="A24" s="26">
+        <v>1</v>
+      </c>
+      <c r="B24" s="26">
+        <v>1</v>
+      </c>
+      <c r="C24" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="37" t="s">
+      <c r="F24" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="27">
         <v>3</v>
       </c>
-      <c r="H24" s="34">
+      <c r="H24" s="29">
         <v>43055</v>
       </c>
-      <c r="I24" s="47">
+      <c r="I24" s="42">
         <v>20</v>
       </c>
-      <c r="J24" s="32">
+      <c r="J24" s="27">
         <v>4</v>
       </c>
-      <c r="K24" s="48">
+      <c r="K24" s="43">
         <v>699</v>
       </c>
-      <c r="L24" s="46" t="s">
+      <c r="L24" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="31">
-        <v>1</v>
-      </c>
-      <c r="B25" s="31">
-        <v>1</v>
-      </c>
-      <c r="C25" s="31" t="s">
+      <c r="A25" s="26">
+        <v>1</v>
+      </c>
+      <c r="B25" s="26">
+        <v>1</v>
+      </c>
+      <c r="C25" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="27">
         <v>3</v>
       </c>
-      <c r="H25" s="34">
+      <c r="H25" s="29">
         <v>43058</v>
       </c>
-      <c r="I25" s="47">
+      <c r="I25" s="42">
         <v>20</v>
       </c>
-      <c r="J25" s="32">
+      <c r="J25" s="27">
         <v>4</v>
       </c>
-      <c r="K25" s="48">
+      <c r="K25" s="43">
         <v>899</v>
       </c>
-      <c r="L25" s="40" t="s">
+      <c r="L25" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="31">
-        <v>1</v>
-      </c>
-      <c r="B26" s="31">
-        <v>1</v>
-      </c>
-      <c r="C26" s="31" t="s">
+      <c r="A26" s="26">
+        <v>1</v>
+      </c>
+      <c r="B26" s="26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="F26" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="27">
         <v>3</v>
       </c>
-      <c r="H26" s="34">
+      <c r="H26" s="29">
         <v>43056</v>
       </c>
-      <c r="I26" s="47">
+      <c r="I26" s="42">
         <v>20</v>
       </c>
-      <c r="J26" s="32">
+      <c r="J26" s="27">
         <v>4</v>
       </c>
-      <c r="K26" s="48">
+      <c r="K26" s="43">
         <v>899</v>
       </c>
-      <c r="L26" s="46" t="s">
+      <c r="L26" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="31">
-        <v>1</v>
-      </c>
-      <c r="B27" s="31">
-        <v>1</v>
-      </c>
-      <c r="C27" s="31" t="s">
+      <c r="A27" s="26">
+        <v>1</v>
+      </c>
+      <c r="B27" s="26">
+        <v>1</v>
+      </c>
+      <c r="C27" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="27">
         <v>3</v>
       </c>
-      <c r="H27" s="34">
+      <c r="H27" s="29">
         <v>43062</v>
       </c>
-      <c r="I27" s="47">
+      <c r="I27" s="42">
         <v>20</v>
       </c>
-      <c r="J27" s="32">
+      <c r="J27" s="27">
         <v>4</v>
       </c>
-      <c r="K27" s="48">
+      <c r="K27" s="43">
         <v>899</v>
       </c>
-      <c r="L27" s="46" t="s">
+      <c r="L27" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="M27" s="46"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="32"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="31">
-        <v>1</v>
-      </c>
-      <c r="B28" s="31">
-        <v>1</v>
-      </c>
-      <c r="C28" s="31" t="s">
+      <c r="A28" s="26">
+        <v>1</v>
+      </c>
+      <c r="B28" s="26">
+        <v>1</v>
+      </c>
+      <c r="C28" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="27">
         <v>3</v>
       </c>
-      <c r="H28" s="34">
+      <c r="H28" s="29">
         <v>43068</v>
       </c>
-      <c r="I28" s="47">
+      <c r="I28" s="42">
         <v>20</v>
       </c>
-      <c r="J28" s="32">
+      <c r="J28" s="27">
         <v>4</v>
       </c>
-      <c r="K28" s="48">
+      <c r="K28" s="43">
         <v>899</v>
       </c>
-      <c r="L28" s="46" t="s">
+      <c r="L28" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="M28" s="46"/>
-      <c r="N28" s="46"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="32"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="31">
-        <v>1</v>
-      </c>
-      <c r="B29" s="31">
-        <v>1</v>
-      </c>
-      <c r="C29" s="31" t="s">
+      <c r="A29" s="26">
+        <v>1</v>
+      </c>
+      <c r="B29" s="26">
+        <v>1</v>
+      </c>
+      <c r="C29" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="37" t="s">
+      <c r="F29" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G29" s="27">
         <v>3</v>
       </c>
-      <c r="H29" s="34">
+      <c r="H29" s="29">
         <v>43054</v>
       </c>
-      <c r="I29" s="47">
+      <c r="I29" s="42">
         <v>20</v>
       </c>
-      <c r="J29" s="32">
+      <c r="J29" s="27">
         <v>4</v>
       </c>
-      <c r="K29" s="48">
+      <c r="K29" s="43">
         <v>699</v>
       </c>
-      <c r="L29" s="46" t="s">
+      <c r="L29" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="31">
-        <v>1</v>
-      </c>
-      <c r="B30" s="31">
-        <v>1</v>
-      </c>
-      <c r="C30" s="31" t="s">
+      <c r="A30" s="26">
+        <v>1</v>
+      </c>
+      <c r="B30" s="26">
+        <v>1</v>
+      </c>
+      <c r="C30" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="F30" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G30" s="32">
+      <c r="G30" s="27">
         <v>3</v>
       </c>
-      <c r="H30" s="34">
+      <c r="H30" s="29">
         <v>43058</v>
       </c>
-      <c r="I30" s="47">
+      <c r="I30" s="42">
         <v>20</v>
       </c>
-      <c r="J30" s="32">
+      <c r="J30" s="27">
         <v>4</v>
       </c>
-      <c r="K30" s="48">
+      <c r="K30" s="43">
         <v>899</v>
       </c>
-      <c r="L30" s="46" t="s">
+      <c r="L30" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="51"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-    </row>
-    <row r="33" spans="1:16" s="33" customFormat="1" ht="30">
-      <c r="A33" s="33" t="s">
+      <c r="B32" s="46"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+    </row>
+    <row r="33" spans="1:16" s="28" customFormat="1" ht="30">
+      <c r="A33" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="33" t="s">
+      <c r="B33" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="28" t="s">
         <v>4</v>
       </c>
       <c r="F33" s="6"/>
@@ -3065,7 +3080,7 @@
       <c r="J33" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="K33" s="49" t="s">
+      <c r="K33" s="44" t="s">
         <v>83</v>
       </c>
       <c r="L33" s="7" t="s">
@@ -3074,546 +3089,558 @@
       <c r="M33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N33" s="49"/>
+      <c r="N33" s="44"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="31">
+      <c r="A34" s="26">
         <v>2</v>
       </c>
-      <c r="B34" s="31">
-        <v>1</v>
-      </c>
-      <c r="C34" s="31" t="s">
+      <c r="B34" s="26">
+        <v>1</v>
+      </c>
+      <c r="C34" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="32" t="s">
+      <c r="F34" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="G34" s="32">
+      <c r="G34" s="27">
         <v>5</v>
       </c>
-      <c r="H34" s="34">
+      <c r="H34" s="29">
         <v>43055</v>
       </c>
-      <c r="I34" s="32">
+      <c r="I34" s="27">
         <v>15</v>
       </c>
-      <c r="J34" s="32">
+      <c r="J34" s="27">
         <v>5</v>
       </c>
-      <c r="K34" s="48">
+      <c r="K34" s="43">
         <v>7999</v>
       </c>
-      <c r="L34" s="46" t="s">
+      <c r="L34" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="M34" s="46"/>
-      <c r="N34" s="46"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="31">
+      <c r="A35" s="26">
         <v>2</v>
       </c>
-      <c r="B35" s="31">
-        <v>1</v>
-      </c>
-      <c r="C35" s="31" t="s">
+      <c r="B35" s="26">
+        <v>1</v>
+      </c>
+      <c r="C35" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="G35" s="32">
+      <c r="G35" s="27">
         <v>5</v>
       </c>
-      <c r="H35" s="34">
+      <c r="H35" s="29">
         <v>43062</v>
       </c>
-      <c r="I35" s="32">
+      <c r="I35" s="27">
         <v>15</v>
       </c>
-      <c r="J35" s="32">
+      <c r="J35" s="27">
         <v>5</v>
       </c>
-      <c r="K35" s="48">
+      <c r="K35" s="43">
         <v>7999</v>
       </c>
-      <c r="L35" s="46" t="s">
+      <c r="L35" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="M35" s="46"/>
-      <c r="N35" s="46"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="31">
+      <c r="A36" s="26">
         <v>2</v>
       </c>
-      <c r="B36" s="31">
+      <c r="B36" s="26">
         <v>6</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="32" t="s">
+      <c r="F36" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G36" s="32">
+      <c r="G36" s="27">
         <v>5</v>
       </c>
-      <c r="H36" s="34">
+      <c r="H36" s="29">
         <v>43056</v>
       </c>
-      <c r="I36" s="32">
+      <c r="I36" s="27">
         <v>15</v>
       </c>
-      <c r="J36" s="32">
+      <c r="J36" s="27">
         <v>5</v>
       </c>
-      <c r="K36" s="48">
+      <c r="K36" s="43">
         <v>7999</v>
       </c>
-      <c r="L36" s="40" t="s">
+      <c r="L36" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="31">
+      <c r="A37" s="26">
         <v>2</v>
       </c>
-      <c r="B37" s="31">
+      <c r="B37" s="26">
         <v>6</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E37" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="32" t="s">
+      <c r="F37" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G37" s="32">
+      <c r="G37" s="27">
         <v>5</v>
       </c>
-      <c r="H37" s="34">
+      <c r="H37" s="29">
         <v>43062</v>
       </c>
-      <c r="I37" s="32">
+      <c r="I37" s="27">
         <v>15</v>
       </c>
-      <c r="J37" s="32">
+      <c r="J37" s="27">
         <v>5</v>
       </c>
-      <c r="K37" s="48">
+      <c r="K37" s="43">
         <v>7999</v>
       </c>
-      <c r="L37" s="40" t="s">
+      <c r="L37" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="31">
+      <c r="A38" s="26">
         <v>2</v>
       </c>
-      <c r="B38" s="31">
+      <c r="B38" s="26">
         <v>6</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G38" s="32">
+      <c r="G38" s="27">
         <v>5</v>
       </c>
-      <c r="H38" s="34">
+      <c r="H38" s="29">
         <v>43072</v>
       </c>
-      <c r="I38" s="32">
+      <c r="I38" s="27">
         <v>15</v>
       </c>
-      <c r="J38" s="32">
+      <c r="J38" s="27">
         <v>5</v>
       </c>
-      <c r="K38" s="48">
+      <c r="K38" s="43">
         <v>8999</v>
       </c>
-      <c r="L38" s="40" t="s">
+      <c r="L38" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="M38" s="46"/>
-      <c r="N38" s="46"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="31">
+      <c r="A39" s="26">
         <v>2</v>
       </c>
-      <c r="C39" s="31" t="s">
+      <c r="B39" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="C39" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="G39" s="32">
+      <c r="G39" s="27">
         <v>6</v>
       </c>
-      <c r="H39" s="34">
+      <c r="H39" s="29">
         <v>43055</v>
       </c>
-      <c r="I39" s="32">
+      <c r="I39" s="27">
         <v>15</v>
       </c>
-      <c r="J39" s="32">
+      <c r="J39" s="27">
         <v>5</v>
       </c>
-      <c r="K39" s="48">
+      <c r="K39" s="43">
         <v>5399</v>
       </c>
-      <c r="L39" s="40" t="s">
+      <c r="L39" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="M39" s="46"/>
-      <c r="N39" s="46"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="31">
+      <c r="A40" s="26">
         <v>2</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="B40" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="C40" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="G40" s="32">
+      <c r="G40" s="27">
         <v>6</v>
       </c>
-      <c r="H40" s="34">
+      <c r="H40" s="29">
         <v>43065</v>
       </c>
-      <c r="I40" s="32">
+      <c r="I40" s="27">
         <v>15</v>
       </c>
-      <c r="J40" s="32">
+      <c r="J40" s="27">
         <v>5</v>
       </c>
-      <c r="K40" s="48">
+      <c r="K40" s="43">
         <v>6399</v>
       </c>
-      <c r="L40" s="46" t="s">
+      <c r="L40" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="M40" s="46"/>
-      <c r="N40" s="46"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="31">
+      <c r="A41" s="26">
         <v>2</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="B41" s="26">
+        <v>8</v>
+      </c>
+      <c r="C41" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E41" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="F41" s="32" t="s">
+      <c r="F41" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="G41" s="32">
+      <c r="G41" s="27">
         <v>7</v>
       </c>
-      <c r="H41" s="34">
+      <c r="H41" s="29">
         <v>43062</v>
       </c>
-      <c r="I41" s="32">
+      <c r="I41" s="27">
         <v>15</v>
       </c>
-      <c r="J41" s="32">
+      <c r="J41" s="27">
         <v>5</v>
       </c>
-      <c r="K41" s="48">
+      <c r="K41" s="43">
         <v>7399</v>
       </c>
-      <c r="L41" s="46" t="s">
+      <c r="L41" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="M41" s="46"/>
-      <c r="N41" s="46"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="31">
+      <c r="A42" s="26">
         <v>2</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="B42" s="26">
+        <v>8</v>
+      </c>
+      <c r="C42" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="D42" s="31" t="s">
+      <c r="D42" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="32" t="s">
+      <c r="F42" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="G42" s="32">
+      <c r="G42" s="27">
         <v>7</v>
       </c>
-      <c r="H42" s="34">
+      <c r="H42" s="29">
         <v>43072</v>
       </c>
-      <c r="I42" s="32">
+      <c r="I42" s="27">
         <v>15</v>
       </c>
-      <c r="J42" s="32">
+      <c r="J42" s="27">
         <v>5</v>
       </c>
-      <c r="K42" s="48">
+      <c r="K42" s="43">
         <v>8399</v>
       </c>
-      <c r="L42" s="40" t="s">
+      <c r="L42" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="M42" s="46"/>
-      <c r="N42" s="46"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="32"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="27"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="31">
+      <c r="A43" s="26">
         <v>2</v>
       </c>
-      <c r="B43" s="31">
+      <c r="B43" s="26">
         <v>3</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="32" t="s">
+      <c r="F43" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="G43" s="32">
+      <c r="G43" s="27">
         <v>6</v>
       </c>
-      <c r="H43" s="34">
+      <c r="H43" s="29">
         <v>43056</v>
       </c>
-      <c r="I43" s="32">
+      <c r="I43" s="27">
         <v>15</v>
       </c>
-      <c r="J43" s="32">
+      <c r="J43" s="27">
         <v>5</v>
       </c>
-      <c r="K43" s="48">
+      <c r="K43" s="43">
         <v>5699</v>
       </c>
-      <c r="L43" s="46" t="s">
+      <c r="L43" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="M43" s="46"/>
-      <c r="N43" s="46"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="41"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="27"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="31">
+      <c r="A44" s="26">
         <v>2</v>
       </c>
-      <c r="B44" s="31">
+      <c r="B44" s="26">
         <v>3</v>
       </c>
-      <c r="C44" s="31" t="s">
+      <c r="C44" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="G44" s="32">
+      <c r="G44" s="27">
         <v>6</v>
       </c>
-      <c r="H44" s="34">
+      <c r="H44" s="29">
         <v>43063</v>
       </c>
-      <c r="I44" s="32">
+      <c r="I44" s="27">
         <v>15</v>
       </c>
-      <c r="J44" s="32">
+      <c r="J44" s="27">
         <v>5</v>
       </c>
-      <c r="K44" s="48">
+      <c r="K44" s="43">
         <v>5699</v>
       </c>
-      <c r="L44" s="46" t="s">
+      <c r="L44" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="M44" s="46"/>
-      <c r="N44" s="46"/>
-      <c r="O44" s="32"/>
-      <c r="P44" s="32"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="27"/>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="31">
+      <c r="A45" s="26">
         <v>2</v>
       </c>
-      <c r="B45" s="31">
+      <c r="B45" s="26">
         <v>3</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="32" t="s">
+      <c r="F45" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="G45" s="32">
+      <c r="G45" s="27">
         <v>6</v>
       </c>
-      <c r="H45" s="34">
+      <c r="H45" s="29">
         <v>43071</v>
       </c>
-      <c r="I45" s="32">
+      <c r="I45" s="27">
         <v>15</v>
       </c>
-      <c r="J45" s="32">
+      <c r="J45" s="27">
         <v>5</v>
       </c>
-      <c r="K45" s="48">
+      <c r="K45" s="43">
         <v>6699</v>
       </c>
-      <c r="L45" s="40" t="s">
+      <c r="L45" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="M45" s="46"/>
-      <c r="N45" s="46"/>
-      <c r="O45" s="32"/>
-      <c r="P45" s="32"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
     </row>
     <row r="46" spans="1:16">
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="46"/>
-      <c r="N46" s="46"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="41"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="27"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="51" t="s">
+      <c r="A47" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="51"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="46"/>
-      <c r="N47" s="46"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-    </row>
-    <row r="48" spans="1:16" s="33" customFormat="1" ht="30">
-      <c r="A48" s="33" t="s">
+      <c r="B47" s="46"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="41"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="41"/>
+      <c r="O47" s="27"/>
+      <c r="P47" s="27"/>
+    </row>
+    <row r="48" spans="1:16" s="28" customFormat="1" ht="30">
+      <c r="A48" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="33" t="s">
+      <c r="B48" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="33" t="s">
+      <c r="D48" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="33" t="s">
+      <c r="E48" s="28" t="s">
         <v>4</v>
       </c>
       <c r="F48" s="6"/>
@@ -3629,7 +3656,7 @@
       <c r="J48" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="K48" s="49" t="s">
+      <c r="K48" s="44" t="s">
         <v>83</v>
       </c>
       <c r="L48" s="7" t="s">
@@ -3638,539 +3665,539 @@
       <c r="M48" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="N48" s="49"/>
+      <c r="N48" s="44"/>
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="31">
+      <c r="A49" s="26">
         <v>3</v>
       </c>
-      <c r="B49" s="31">
-        <v>1</v>
-      </c>
-      <c r="C49" s="31" t="s">
+      <c r="B49" s="26">
+        <v>1</v>
+      </c>
+      <c r="C49" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="F49" s="32" t="s">
+      <c r="F49" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="G49" s="32">
+      <c r="G49" s="27">
         <v>4</v>
       </c>
-      <c r="H49" s="34">
+      <c r="H49" s="29">
         <v>43053</v>
       </c>
-      <c r="I49" s="32">
+      <c r="I49" s="27">
         <v>10</v>
       </c>
-      <c r="J49" s="32">
+      <c r="J49" s="27">
         <v>4</v>
       </c>
-      <c r="K49" s="48">
+      <c r="K49" s="43">
         <v>2399</v>
       </c>
-      <c r="L49" s="46" t="s">
+      <c r="L49" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="M49" s="46"/>
-      <c r="N49" s="46"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
+      <c r="M49" s="41"/>
+      <c r="N49" s="41"/>
+      <c r="O49" s="27"/>
+      <c r="P49" s="27"/>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="31">
+      <c r="A50" s="26">
         <v>3</v>
       </c>
-      <c r="B50" s="31">
-        <v>1</v>
-      </c>
-      <c r="C50" s="31" t="s">
+      <c r="B50" s="26">
+        <v>1</v>
+      </c>
+      <c r="C50" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="D50" s="31" t="s">
+      <c r="D50" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E50" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="F50" s="32" t="s">
+      <c r="F50" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="G50" s="32">
+      <c r="G50" s="27">
         <v>4</v>
       </c>
-      <c r="H50" s="34">
+      <c r="H50" s="29">
         <v>43062</v>
       </c>
-      <c r="I50" s="32">
+      <c r="I50" s="27">
         <v>10</v>
       </c>
-      <c r="J50" s="32">
+      <c r="J50" s="27">
         <v>4</v>
       </c>
-      <c r="K50" s="48">
+      <c r="K50" s="43">
         <v>2399</v>
       </c>
-      <c r="L50" s="46" t="s">
+      <c r="L50" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="M50" s="46"/>
-      <c r="N50" s="46"/>
-      <c r="O50" s="32"/>
-      <c r="P50" s="32"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="41"/>
+      <c r="O50" s="27"/>
+      <c r="P50" s="27"/>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="31">
+      <c r="A51" s="26">
         <v>3</v>
       </c>
-      <c r="B51" s="31">
+      <c r="B51" s="26">
         <v>7</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C51" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="D51" s="31" t="s">
+      <c r="D51" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="E51" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="F51" s="32" t="s">
+      <c r="F51" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="G51" s="32">
+      <c r="G51" s="27">
         <v>5</v>
       </c>
-      <c r="H51" s="34">
+      <c r="H51" s="29">
         <v>43053</v>
       </c>
-      <c r="I51" s="32">
+      <c r="I51" s="27">
         <v>10</v>
       </c>
-      <c r="J51" s="32">
+      <c r="J51" s="27">
         <v>4</v>
       </c>
-      <c r="K51" s="48">
+      <c r="K51" s="43">
         <v>2999</v>
       </c>
-      <c r="L51" s="40" t="s">
+      <c r="L51" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="M51" s="46"/>
-      <c r="N51" s="46"/>
-      <c r="O51" s="32"/>
-      <c r="P51" s="32"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="27"/>
+      <c r="P51" s="27"/>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="31">
+      <c r="A52" s="26">
         <v>3</v>
       </c>
-      <c r="B52" s="31">
+      <c r="B52" s="26">
         <v>7</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C52" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D52" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E52" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="F52" s="32" t="s">
+      <c r="F52" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="G52" s="32">
+      <c r="G52" s="27">
         <v>5</v>
       </c>
-      <c r="H52" s="34">
+      <c r="H52" s="29">
         <v>43064</v>
       </c>
-      <c r="I52" s="32">
+      <c r="I52" s="27">
         <v>10</v>
       </c>
-      <c r="J52" s="32">
+      <c r="J52" s="27">
         <v>4</v>
       </c>
-      <c r="K52" s="48">
+      <c r="K52" s="43">
         <v>3999</v>
       </c>
-      <c r="L52" s="40" t="s">
+      <c r="L52" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="M52" s="46"/>
-      <c r="N52" s="46"/>
-      <c r="O52" s="32"/>
-      <c r="P52" s="32"/>
+      <c r="M52" s="41"/>
+      <c r="N52" s="41"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="27"/>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="31">
+      <c r="A53" s="26">
         <v>3</v>
       </c>
-      <c r="B53" s="31">
+      <c r="B53" s="26">
         <v>5</v>
       </c>
-      <c r="C53" s="31" t="s">
+      <c r="C53" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D53" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E53" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="32" t="s">
+      <c r="F53" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="G53" s="32">
+      <c r="G53" s="27">
         <v>5</v>
       </c>
-      <c r="H53" s="34">
+      <c r="H53" s="29">
         <v>43053</v>
       </c>
-      <c r="I53" s="32">
+      <c r="I53" s="27">
         <v>10</v>
       </c>
-      <c r="J53" s="32">
+      <c r="J53" s="27">
         <v>4</v>
       </c>
-      <c r="K53" s="48">
+      <c r="K53" s="43">
         <v>3699</v>
       </c>
-      <c r="L53" s="46" t="s">
+      <c r="L53" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="M53" s="46"/>
-      <c r="N53" s="46"/>
-      <c r="O53" s="32"/>
-      <c r="P53" s="32"/>
+      <c r="M53" s="41"/>
+      <c r="N53" s="41"/>
+      <c r="O53" s="27"/>
+      <c r="P53" s="27"/>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="31">
+      <c r="A54" s="26">
         <v>3</v>
       </c>
-      <c r="B54" s="31">
+      <c r="B54" s="26">
         <v>5</v>
       </c>
-      <c r="C54" s="31" t="s">
+      <c r="C54" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="31" t="s">
+      <c r="D54" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E54" s="31" t="s">
+      <c r="E54" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F54" s="32" t="s">
+      <c r="F54" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="G54" s="32">
+      <c r="G54" s="27">
         <v>5</v>
       </c>
-      <c r="H54" s="34">
+      <c r="H54" s="29">
         <v>43057</v>
       </c>
-      <c r="I54" s="32">
+      <c r="I54" s="27">
         <v>10</v>
       </c>
-      <c r="J54" s="32">
+      <c r="J54" s="27">
         <v>4</v>
       </c>
-      <c r="K54" s="48">
+      <c r="K54" s="43">
         <v>4699</v>
       </c>
-      <c r="L54" s="40" t="s">
+      <c r="L54" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="M54" s="46"/>
-      <c r="N54" s="46"/>
-      <c r="O54" s="32"/>
-      <c r="P54" s="32"/>
+      <c r="M54" s="41"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="27"/>
+      <c r="P54" s="27"/>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="31">
+      <c r="A55" s="26">
         <v>3</v>
       </c>
-      <c r="B55" s="31">
+      <c r="B55" s="26">
         <v>3</v>
       </c>
-      <c r="C55" s="31" t="s">
+      <c r="C55" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="D55" s="31" t="s">
+      <c r="D55" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E55" s="31" t="s">
+      <c r="E55" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="32" t="s">
+      <c r="F55" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="G55" s="32">
+      <c r="G55" s="27">
         <v>4</v>
       </c>
-      <c r="H55" s="34">
+      <c r="H55" s="29">
         <v>43055</v>
       </c>
-      <c r="I55" s="32">
+      <c r="I55" s="27">
         <v>10</v>
       </c>
-      <c r="J55" s="32">
+      <c r="J55" s="27">
         <v>4</v>
       </c>
-      <c r="K55" s="48">
+      <c r="K55" s="43">
         <v>1999</v>
       </c>
-      <c r="L55" s="46" t="s">
+      <c r="L55" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="M55" s="46"/>
-      <c r="N55" s="46"/>
-      <c r="O55" s="32"/>
-      <c r="P55" s="32"/>
+      <c r="M55" s="41"/>
+      <c r="N55" s="41"/>
+      <c r="O55" s="27"/>
+      <c r="P55" s="27"/>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="31">
+      <c r="A56" s="26">
         <v>3</v>
       </c>
-      <c r="B56" s="31">
+      <c r="B56" s="26">
         <v>3</v>
       </c>
-      <c r="C56" s="31" t="s">
+      <c r="C56" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="D56" s="31" t="s">
+      <c r="D56" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E56" s="31" t="s">
+      <c r="E56" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F56" s="32" t="s">
+      <c r="F56" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="G56" s="32">
+      <c r="G56" s="27">
         <v>4</v>
       </c>
-      <c r="H56" s="34">
+      <c r="H56" s="29">
         <v>43063</v>
       </c>
-      <c r="I56" s="32">
+      <c r="I56" s="27">
         <v>10</v>
       </c>
-      <c r="J56" s="32">
+      <c r="J56" s="27">
         <v>4</v>
       </c>
-      <c r="K56" s="48">
+      <c r="K56" s="43">
         <v>1999</v>
       </c>
-      <c r="L56" s="46" t="s">
+      <c r="L56" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="M56" s="46"/>
-      <c r="N56" s="46"/>
-      <c r="O56" s="32"/>
-      <c r="P56" s="32"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
     </row>
     <row r="57" spans="1:16">
-      <c r="A57" s="31">
+      <c r="A57" s="26">
         <v>3</v>
       </c>
-      <c r="B57" s="31">
+      <c r="B57" s="26">
         <v>3</v>
       </c>
-      <c r="C57" s="31" t="s">
+      <c r="C57" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="D57" s="31" t="s">
+      <c r="D57" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E57" s="31" t="s">
+      <c r="E57" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F57" s="32" t="s">
+      <c r="F57" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="G57" s="32">
+      <c r="G57" s="27">
         <v>4</v>
       </c>
-      <c r="H57" s="34">
+      <c r="H57" s="29">
         <v>43064</v>
       </c>
-      <c r="I57" s="32">
+      <c r="I57" s="27">
         <v>10</v>
       </c>
-      <c r="J57" s="32">
+      <c r="J57" s="27">
         <v>4</v>
       </c>
-      <c r="K57" s="48">
+      <c r="K57" s="43">
         <v>2999</v>
       </c>
-      <c r="L57" s="46" t="s">
+      <c r="L57" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="M57" s="46"/>
-      <c r="N57" s="46"/>
-      <c r="O57" s="32"/>
-      <c r="P57" s="32"/>
+      <c r="M57" s="41"/>
+      <c r="N57" s="41"/>
+      <c r="O57" s="27"/>
+      <c r="P57" s="27"/>
     </row>
     <row r="58" spans="1:16">
-      <c r="A58" s="31">
+      <c r="A58" s="26">
         <v>3</v>
       </c>
-      <c r="B58" s="31">
-        <v>1</v>
-      </c>
-      <c r="C58" s="31" t="s">
+      <c r="B58" s="26">
+        <v>1</v>
+      </c>
+      <c r="C58" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E58" s="31" t="s">
+      <c r="E58" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="F58" s="32" t="s">
+      <c r="F58" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="G58" s="32">
+      <c r="G58" s="27">
         <v>7</v>
       </c>
-      <c r="H58" s="34">
+      <c r="H58" s="29">
         <v>43052</v>
       </c>
-      <c r="I58" s="32">
+      <c r="I58" s="27">
         <v>10</v>
       </c>
-      <c r="J58" s="32">
+      <c r="J58" s="27">
         <v>4</v>
       </c>
-      <c r="K58" s="48">
+      <c r="K58" s="43">
         <v>3999</v>
       </c>
-      <c r="L58" s="46" t="s">
+      <c r="L58" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="M58" s="46"/>
-      <c r="N58" s="46"/>
-      <c r="O58" s="32"/>
-      <c r="P58" s="32"/>
+      <c r="M58" s="41"/>
+      <c r="N58" s="41"/>
+      <c r="O58" s="27"/>
+      <c r="P58" s="27"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="31">
+      <c r="A59" s="26">
         <v>3</v>
       </c>
-      <c r="B59" s="31">
-        <v>1</v>
-      </c>
-      <c r="C59" s="31" t="s">
+      <c r="B59" s="26">
+        <v>1</v>
+      </c>
+      <c r="C59" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="D59" s="31" t="s">
+      <c r="D59" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E59" s="31" t="s">
+      <c r="E59" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="F59" s="32" t="s">
+      <c r="F59" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="G59" s="32">
+      <c r="G59" s="27">
         <v>7</v>
       </c>
-      <c r="H59" s="34">
+      <c r="H59" s="29">
         <v>43054</v>
       </c>
-      <c r="I59" s="32">
+      <c r="I59" s="27">
         <v>10</v>
       </c>
-      <c r="J59" s="32">
+      <c r="J59" s="27">
         <v>4</v>
       </c>
-      <c r="K59" s="48">
+      <c r="K59" s="43">
         <v>3999</v>
       </c>
-      <c r="L59" s="46" t="s">
+      <c r="L59" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="M59" s="46"/>
-      <c r="N59" s="46"/>
-      <c r="O59" s="32"/>
-      <c r="P59" s="32"/>
+      <c r="M59" s="41"/>
+      <c r="N59" s="41"/>
+      <c r="O59" s="27"/>
+      <c r="P59" s="27"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="31">
+      <c r="A60" s="26">
         <v>3</v>
       </c>
-      <c r="B60" s="31">
-        <v>1</v>
-      </c>
-      <c r="C60" s="31" t="s">
+      <c r="B60" s="26">
+        <v>1</v>
+      </c>
+      <c r="C60" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D60" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E60" s="31" t="s">
+      <c r="E60" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="F60" s="32" t="s">
+      <c r="F60" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="G60" s="32">
+      <c r="G60" s="27">
         <v>7</v>
       </c>
-      <c r="H60" s="34">
+      <c r="H60" s="29">
         <v>43057</v>
       </c>
-      <c r="I60" s="32">
+      <c r="I60" s="27">
         <v>10</v>
       </c>
-      <c r="J60" s="32">
+      <c r="J60" s="27">
         <v>4</v>
       </c>
-      <c r="K60" s="48">
+      <c r="K60" s="43">
         <v>4999</v>
       </c>
-      <c r="L60" s="46" t="s">
+      <c r="L60" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="M60" s="46"/>
-      <c r="N60" s="46"/>
-      <c r="O60" s="32"/>
-      <c r="P60" s="32"/>
+      <c r="M60" s="41"/>
+      <c r="N60" s="41"/>
+      <c r="O60" s="27"/>
+      <c r="P60" s="27"/>
     </row>
     <row r="61" spans="1:16">
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="32"/>
-      <c r="J61" s="32"/>
-      <c r="K61" s="46"/>
-      <c r="L61" s="46"/>
-      <c r="M61" s="46"/>
-      <c r="N61" s="46"/>
-      <c r="O61" s="32"/>
-      <c r="P61" s="32"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="41"/>
+      <c r="L61" s="41"/>
+      <c r="M61" s="41"/>
+      <c r="N61" s="41"/>
+      <c r="O61" s="27"/>
+      <c r="P61" s="27"/>
     </row>
     <row r="62" spans="1:16">
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="32"/>
-      <c r="J62" s="32"/>
-      <c r="K62" s="46"/>
-      <c r="L62" s="46"/>
-      <c r="M62" s="46"/>
-      <c r="N62" s="46"/>
-      <c r="O62" s="32"/>
-      <c r="P62" s="32"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
+      <c r="I62" s="27"/>
+      <c r="J62" s="27"/>
+      <c r="K62" s="41"/>
+      <c r="L62" s="41"/>
+      <c r="M62" s="41"/>
+      <c r="N62" s="41"/>
+      <c r="O62" s="27"/>
+      <c r="P62" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6457,250 +6484,262 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="26"/>
+    <col min="1" max="16384" width="9" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="51" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="51" t="s">
         <v>331</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="51" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="30">
-        <v>1</v>
-      </c>
-      <c r="B2" s="30">
-        <v>1</v>
-      </c>
-      <c r="C2" s="27" t="s">
+      <c r="A2" s="51">
+        <v>1</v>
+      </c>
+      <c r="B2" s="51">
+        <v>1</v>
+      </c>
+      <c r="C2" s="52" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="30">
-        <v>1</v>
-      </c>
-      <c r="B3" s="30">
+      <c r="A3" s="51">
+        <v>1</v>
+      </c>
+      <c r="B3" s="51">
         <v>2</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="52" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="30">
-        <v>1</v>
-      </c>
-      <c r="B4" s="30">
+      <c r="A4" s="51">
+        <v>1</v>
+      </c>
+      <c r="B4" s="51">
         <v>3</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="53" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="30">
-        <v>1</v>
-      </c>
-      <c r="B5" s="30">
+      <c r="A5" s="51">
+        <v>1</v>
+      </c>
+      <c r="B5" s="51">
         <v>4</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="52" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="30">
-        <v>1</v>
-      </c>
-      <c r="B6" s="30">
+      <c r="A6" s="51">
+        <v>1</v>
+      </c>
+      <c r="B6" s="51">
         <v>5</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="53" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="30">
-        <v>1</v>
-      </c>
-      <c r="B7" s="30">
+      <c r="A7" s="51">
+        <v>1</v>
+      </c>
+      <c r="B7" s="51">
         <v>6</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="53" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A8" s="30">
+      <c r="A8" s="51">
         <v>2</v>
       </c>
-      <c r="B8" s="30">
-        <v>1</v>
-      </c>
-      <c r="C8" s="29" t="s">
+      <c r="B8" s="51">
+        <v>1</v>
+      </c>
+      <c r="C8" s="54" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="30">
+      <c r="A9" s="51">
         <v>2</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="51">
         <v>2</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="51" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="30">
+      <c r="A10" s="51">
         <v>2</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="51">
         <v>3</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="51" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="30">
+      <c r="A11" s="51">
         <v>2</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="51">
         <v>4</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="51" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="30">
+      <c r="A12" s="51">
         <v>2</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="51">
         <v>5</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="51" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="30">
+      <c r="A13" s="51">
         <v>2</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="51">
         <v>6</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="51" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="30">
+      <c r="A14" s="51">
         <v>2</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="51">
         <v>7</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="51" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="26">
+      <c r="A15" s="51">
+        <v>2</v>
+      </c>
+      <c r="B15" s="51">
+        <v>8</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="51">
         <v>3</v>
       </c>
-      <c r="B15" s="26">
-        <v>1</v>
-      </c>
-      <c r="C15" s="26" t="s">
+      <c r="B16" s="51">
+        <v>1</v>
+      </c>
+      <c r="C16" s="51" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="26">
+    <row r="17" spans="1:3">
+      <c r="A17" s="51">
         <v>3</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B17" s="51">
         <v>2</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C17" s="51" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="26">
+    <row r="18" spans="1:3">
+      <c r="A18" s="51">
         <v>3</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B18" s="51">
         <v>3</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C18" s="51" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="26">
+    <row r="19" spans="1:3">
+      <c r="A19" s="51">
         <v>3</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B19" s="51">
         <v>4</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C19" s="51" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="26">
+    <row r="20" spans="1:3">
+      <c r="A20" s="51">
         <v>3</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B20" s="51">
         <v>5</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C20" s="51" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="26">
+    <row r="21" spans="1:3">
+      <c r="A21" s="51">
         <v>3</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B21" s="51">
         <v>6</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C21" s="51" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="26">
+    <row r="22" spans="1:3">
+      <c r="A22" s="51">
         <v>3</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B22" s="51">
         <v>7</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C22" s="51" t="s">
         <v>351</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6727,20 +6766,20 @@
       <c r="B1" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="24">
@@ -6749,20 +6788,20 @@
       <c r="B2" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="47" t="s">
         <v>250</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
     </row>
     <row r="3" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="24">
@@ -6771,20 +6810,20 @@
       <c r="B3" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="48" t="s">
         <v>254</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
     </row>
     <row r="4" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="24">
@@ -6793,20 +6832,20 @@
       <c r="B4" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="49" t="s">
         <v>253</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
     </row>
     <row r="5" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="24">
@@ -6815,20 +6854,20 @@
       <c r="B5" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="24">
@@ -6837,20 +6876,20 @@
       <c r="B6" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="47" t="s">
         <v>256</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="24">
@@ -6859,20 +6898,20 @@
       <c r="B7" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="47" t="s">
         <v>257</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="24">
@@ -6881,20 +6920,20 @@
       <c r="B8" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="24">
@@ -6903,20 +6942,20 @@
       <c r="B9" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="47" t="s">
         <v>259</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
     </row>
     <row r="10" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="24">
@@ -6925,20 +6964,20 @@
       <c r="B10" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="47" t="s">
         <v>260</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
     </row>
     <row r="11" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="24">
@@ -6947,20 +6986,20 @@
       <c r="B11" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="47" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
     </row>
     <row r="12" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="24">
@@ -6969,20 +7008,20 @@
       <c r="B12" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="47" t="s">
         <v>262</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="13" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="24">
@@ -6991,20 +7030,20 @@
       <c r="B13" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="47" t="s">
         <v>263</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
     </row>
     <row r="14" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="24">
@@ -7013,23 +7052,29 @@
       <c r="B14" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="47" t="s">
         <v>264</v>
       </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="C2:N2"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C5:N5"/>
     <mergeCell ref="C13:N13"/>
     <mergeCell ref="C14:N14"/>
     <mergeCell ref="C7:N7"/>
@@ -7038,12 +7083,6 @@
     <mergeCell ref="C10:N10"/>
     <mergeCell ref="C11:N11"/>
     <mergeCell ref="C12:N12"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="C2:N2"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="C4:N4"/>
-    <mergeCell ref="C5:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>